<commit_message>
Completed passing tests for 306 examples.
</commit_message>
<xml_diff>
--- a/data/ClueLayout306.xlsx
+++ b/data/ClueLayout306.xlsx
@@ -3,22 +3,27 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{81B29239-BD82-45AD-BC9C-86C5B4AA0A61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caleb\OneDrive\College\Mines\20-21\Fall 20\CSCI 306-C\eclipse-workspace\ClueGame\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:801_{29C8F885-7D84-4BFC-BFE5-5154029ED251}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{481D1C3A-888A-4C14-BEC6-6267E95C73AB}"/>
   <bookViews>
-    <workbookView xWindow="4155" yWindow="4155" windowWidth="17640" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ClueLayout" sheetId="1" r:id="rId1"/>
     <sheet name="csv" sheetId="3" r:id="rId2"/>
     <sheet name="Test" sheetId="4" r:id="rId3"/>
+    <sheet name="Test (2)" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:AC17"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1806" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2412" uniqueCount="43">
   <si>
     <t>C</t>
   </si>
@@ -290,7 +295,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="46">
+  <fills count="47">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -548,6 +553,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -724,7 +735,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -761,6 +772,9 @@
     <xf numFmtId="0" fontId="0" fillId="44" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="44" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="45" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="46" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1147,8 +1161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="X24" sqref="X24"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5043,14 +5057,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{273E5100-B0A3-4FB2-ADFD-C3D019FF5F92}">
   <dimension ref="A1:AA30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AA20" sqref="AA20"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="24" width="3.7109375" customWidth="1"/>
     <col min="25" max="25" width="4.5703125" customWidth="1"/>
+    <col min="27" max="27" width="40.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
@@ -7085,4 +7100,2054 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFD1785F-39F0-431D-AE91-CA620AE815F0}">
+  <dimension ref="A1:AA30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="24" width="3.7109375" customWidth="1"/>
+    <col min="25" max="25" width="4.5703125" customWidth="1"/>
+    <col min="27" max="27" width="40.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y1" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="U2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="V2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="W2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="X2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y2" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="S3" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="V3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="W3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="X3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y3" s="3">
+        <v>2</v>
+      </c>
+      <c r="AA3" s="22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="S4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="U4" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="V4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="W4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="X4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y4" s="3">
+        <v>3</v>
+      </c>
+      <c r="AA4" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="S5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="T5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="U5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="V5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="W5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="X5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y5" s="3">
+        <v>4</v>
+      </c>
+      <c r="AA5" s="25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="S6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="T6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="U6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="V6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="W6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="X6" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y6" s="3">
+        <v>5</v>
+      </c>
+      <c r="AA6" s="27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="R7" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="V7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="W7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="X7" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y7" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L8" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P8" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R8" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T8" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="U8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="V8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="W8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="M9" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="N9" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O9" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="R9" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="S9" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="T9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="U9" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="V9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="W9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="X9" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y9" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="N10" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O10" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="P10" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="R10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="S10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="T10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="U10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="V10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="W10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y10" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="L11" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="M11" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="N11" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="P11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="R11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="S11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="T11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="U11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="V11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="W11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y11" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="M12" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="N12" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="P12" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="R12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="S12" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="T12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="U12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="V12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="W12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y12" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="L13" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="M13" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="N13" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O13" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="P13" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="R13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="S13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="T13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="U13" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="V13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="W13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y13" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="L14" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="N14" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="P14" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="R14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="S14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="T14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="U14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="V14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="W14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y14" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="K15" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="L15" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="M15" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="N15" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O15" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="P15" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="R15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="S15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="T15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="U15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="V15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="W15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y15" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="O16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="P16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="R16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="S16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="T16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="U16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="V16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="W16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y16" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J17" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="O17" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="P17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="R17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="S17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="T17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="U17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="V17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="W17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="X17" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y17" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M18" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N18" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="O18" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="P18" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q18" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="R18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="S18" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="T18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="U18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="V18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="W18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="X18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y18" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N19" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="O19" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="P19" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="R19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="S19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="T19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="U19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="V19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="W19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="X19" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y19" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F20" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="H20" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K20" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="L20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="O20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="P20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q20" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="R20" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="S20" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="T20" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="U20" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="V20" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="W20" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="X20" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y20" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L21" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="M21" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N21" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="O21" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="P21" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q21" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="R21" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="S21" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="T21" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="U21" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="V21" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="W21" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="X21" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y21" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L22" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M22" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N22" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="O22" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="P22" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q22" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="R22" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="S22" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="T22" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="U22" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="V22" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="W22" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="X22" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y22" s="3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K23" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="L23" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="M23" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="N23" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="O23" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="P23" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q23" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="R23" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="S23" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="T23" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="U23" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="V23" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="W23" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="X23" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y23" s="3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="R24" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="S24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="T24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="U24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="V24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="W24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="X24" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y24" s="3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I25" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K25" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="L25" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="M25" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="N25" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="O25" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="P25" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q25" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="R25" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="S25" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="T25" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="U25" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="V25" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="W25" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="X25" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y25" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="13">
+        <v>0</v>
+      </c>
+      <c r="B26" s="3">
+        <v>1</v>
+      </c>
+      <c r="C26" s="3">
+        <v>2</v>
+      </c>
+      <c r="D26" s="3">
+        <v>3</v>
+      </c>
+      <c r="E26" s="3">
+        <v>4</v>
+      </c>
+      <c r="F26" s="3">
+        <v>5</v>
+      </c>
+      <c r="G26" s="3">
+        <v>6</v>
+      </c>
+      <c r="H26" s="3">
+        <v>7</v>
+      </c>
+      <c r="I26" s="3">
+        <v>8</v>
+      </c>
+      <c r="J26" s="3">
+        <v>9</v>
+      </c>
+      <c r="K26" s="3">
+        <v>10</v>
+      </c>
+      <c r="L26" s="3">
+        <v>11</v>
+      </c>
+      <c r="M26" s="3">
+        <v>12</v>
+      </c>
+      <c r="N26" s="3">
+        <v>13</v>
+      </c>
+      <c r="O26" s="3">
+        <v>14</v>
+      </c>
+      <c r="P26" s="3">
+        <v>15</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>16</v>
+      </c>
+      <c r="R26" s="3">
+        <v>17</v>
+      </c>
+      <c r="S26" s="3">
+        <v>18</v>
+      </c>
+      <c r="T26" s="3">
+        <v>19</v>
+      </c>
+      <c r="U26" s="3">
+        <v>20</v>
+      </c>
+      <c r="V26" s="3">
+        <v>21</v>
+      </c>
+      <c r="W26" s="3">
+        <v>22</v>
+      </c>
+      <c r="X26" s="3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>